<commit_message>
New Strategy function to be tested
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Programming\PomBot\PomBot-TraderRobot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E088E786-DB5F-40F2-BF07-FC6B5F7D8E73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A07640D-7744-4808-B8F9-E5A7998178A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7065" yWindow="-14625" windowWidth="13500" windowHeight="11505" xr2:uid="{0C989F92-7D77-4499-8348-85EE8BE2D94B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0C989F92-7D77-4499-8348-85EE8BE2D94B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>UPMean</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>RSI</t>
+  </si>
+  <si>
+    <t>Periods</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Default</t>
   </si>
 </sst>
 </file>
@@ -58,12 +70,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,11 +96,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,227 +416,540 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCABD38-149A-4E21-B305-86DD041644A1}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>5576</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5578</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5570</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5572</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>5574</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>5572</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>5574</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>5572</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>5570</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>5568</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>5566</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <v>5564</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>5562</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>5560</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <v>5558</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19">
-        <v>5554</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>5552</v>
+        <v>5360</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>5362</v>
+      </c>
+      <c r="C3">
+        <f>IF(B3-A2&gt;0,B3-A2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>5364</v>
+      </c>
+      <c r="C4">
+        <f>IF(B4-B3&gt;0,B4-B3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <f>IF(B4-B3&lt;0,ABS(B4-B3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>5360</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C26" si="0">IF(B5-B4&gt;0,B5-B4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D26" si="1">IF(B5-B4&lt;0,ABS(B5-B4),0)</f>
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>5358</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>5356</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>5360</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>5362</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>5358</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>5356</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>5354</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <v>5352</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>5356</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>5358</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>5354</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>5352</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>5350</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>5348</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>5346</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D20">
-        <f>SUM(A1:A20)/20</f>
-        <v>1114.8</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="E20">
-        <f>SUM(B8:B20)/20</f>
-        <v>3617.3</v>
-      </c>
-      <c r="F20">
-        <f>D20/E20</f>
-        <v>0.30818566334006026</v>
-      </c>
-      <c r="G20">
-        <f>100-100/(1+F20)</f>
-        <v>23.558251093594805</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>5556</v>
-      </c>
-      <c r="B21">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>5344</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D21">
-        <f>(A21+D20*19)/20</f>
-        <v>1336.8600000000001</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="E21">
-        <f>(B21+E20*19)/20</f>
-        <v>3436.4349999999999</v>
-      </c>
-      <c r="F21">
-        <f>D21/E21</f>
-        <v>0.38902525436971752</v>
-      </c>
-      <c r="G21">
-        <f>100-100/(1+F21)</f>
-        <v>28.007068492519323</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>5348</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>19</v>
+      </c>
+      <c r="F22">
+        <f>SUM(C3:C22)/20</f>
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <f>SUM(D3:D22)/20</f>
+        <v>1.6</v>
+      </c>
+      <c r="H22">
+        <f>F22/G22</f>
+        <v>0.625</v>
+      </c>
+      <c r="I22">
+        <f>100-100/(1+H22)</f>
+        <v>38.46153846153846</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>5350</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>20</v>
+      </c>
+      <c r="F23">
+        <f>(F22*19+C23)/20</f>
+        <v>1.05</v>
+      </c>
+      <c r="G23">
+        <f>(G22*19+D23)/20</f>
+        <v>1.52</v>
+      </c>
+      <c r="H23">
+        <f>F23/G23</f>
+        <v>0.69078947368421051</v>
+      </c>
+      <c r="I23">
+        <f>100-(100/(1+H23))</f>
+        <v>40.856031128404673</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>5352</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>21</v>
+      </c>
+      <c r="F24">
+        <f>(F23*19+C24)/20</f>
+        <v>1.0974999999999999</v>
+      </c>
+      <c r="G24">
+        <f>(G23*19+D24)/20</f>
+        <v>1.444</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ref="H24:H26" si="2">F24/G24</f>
+        <v>0.76004155124653738</v>
+      </c>
+      <c r="I24">
+        <f t="shared" ref="I24:I26" si="3">100-100/(1+H24)</f>
+        <v>43.183159551445996</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>5354</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>22</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ref="F24:F26" si="4">(F24*19+C25)/20</f>
+        <v>1.142625</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ref="G24:G26" si="5">(G24*19+D25)/20</f>
+        <v>1.3717999999999999</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>0.8329384749963552</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>45.442795072432062</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>5356</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>23</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="4"/>
+        <v>1.18549375</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="5"/>
+        <v>1.30321</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>0.90967207894353175</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="3"/>
+        <v>47.634988696424799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New method add to be tested
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Programming\PomBot\PomBot-TraderRobot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A07640D-7744-4808-B8F9-E5A7998178A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499D09DB-18E0-4DD5-B147-4623FE528D61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0C989F92-7D77-4499-8348-85EE8BE2D94B}"/>
+    <workbookView xWindow="14655" yWindow="-14775" windowWidth="13500" windowHeight="11505" xr2:uid="{0C989F92-7D77-4499-8348-85EE8BE2D94B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCABD38-149A-4E21-B305-86DD041644A1}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,11 +904,11 @@
         <v>22</v>
       </c>
       <c r="F25">
-        <f t="shared" ref="F24:F26" si="4">(F24*19+C25)/20</f>
+        <f t="shared" ref="F25:F26" si="4">(F24*19+C25)/20</f>
         <v>1.142625</v>
       </c>
       <c r="G25">
-        <f t="shared" ref="G24:G26" si="5">(G24*19+D25)/20</f>
+        <f t="shared" ref="G25:G26" si="5">(G24*19+D25)/20</f>
         <v>1.3717999999999999</v>
       </c>
       <c r="H25">

</xml_diff>

<commit_message>
Bot 01 form and implementation completed
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Programming\PomBot\PomBot-TraderRobot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F86CAD4-10C8-47FC-99BA-27C54F1716FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FC2FD6-3329-4FC0-BA40-8C68D6CE41F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14655" yWindow="-14775" windowWidth="13500" windowHeight="11505" xr2:uid="{0C989F92-7D77-4499-8348-85EE8BE2D94B}"/>
+    <workbookView xWindow="28680" yWindow="-14220" windowWidth="18240" windowHeight="28590" xr2:uid="{0C989F92-7D77-4499-8348-85EE8BE2D94B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCABD38-149A-4E21-B305-86DD041644A1}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>